<commit_message>
update readme, add mc dropout
</commit_message>
<xml_diff>
--- a/doc/simulation_params_range.xlsx
+++ b/doc/simulation_params_range.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\789176_3_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/67802_2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1C696C-EAB1-46BA-9A69-817FF055F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{3D1C696C-EAB1-46BA-9A69-817FF055F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{186B776E-11AB-449A-9FAD-E48E6BF7E0ED}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
+    <workbookView xWindow="2550" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
   <si>
     <t>N</t>
   </si>
@@ -188,9 +188,6 @@
     <t>shape parameter for sweep-linked deleterious mutation DFE</t>
   </si>
   <si>
-    <t>UNIF(100 - 10,000)</t>
-  </si>
-  <si>
     <t>UNIF(0 - 1)</t>
   </si>
   <si>
@@ -203,15 +200,6 @@
     <t>if growing: UNIF(1.5 - 2)*N ; if shrinking: 1/UNIF(1.5-2)*N ; if 2-cycling: UNIF() ; if chaotic: UNIF()</t>
   </si>
   <si>
-    <t>UNIF(0 - 0.25)</t>
-  </si>
-  <si>
-    <t>UNIF(0.75 - 1)</t>
-  </si>
-  <si>
-    <t>UNIF(1 - 4)</t>
-  </si>
-  <si>
     <t>1 - B - U</t>
   </si>
   <si>
@@ -248,10 +236,46 @@
     <t>The range we can search will mainly be determined by my level of patience</t>
   </si>
   <si>
-    <t>10^UNIF(0, 2)/N</t>
-  </si>
-  <si>
-    <t>Ensures all s &gt; 1/N</t>
+    <t>Ensures about half of coefficients are s &lt; 1/N and the other half are s &gt; 1/N</t>
+  </si>
+  <si>
+    <t>0.5: 10^UNIF(-3, 0)/N ; 0.5: 10^UNIF(0,3)/N or 10^UNIF(-3,3)/N</t>
+  </si>
+  <si>
+    <t>0.5: 0; 0.5:UNIF(0-1)</t>
+  </si>
+  <si>
+    <t>0.5: 0; 0.5: UNIF(0, 0.01)</t>
+  </si>
+  <si>
+    <t>0.5: 0; 0.5: UNIF(0, 0.04)</t>
+  </si>
+  <si>
+    <t>10^UNIF(0 - 2)</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>time between observation and sweep fixation</t>
+  </si>
+  <si>
+    <t>10^UNIF(0-3)</t>
+  </si>
+  <si>
+    <t>0.5: 1; 0.5: sample(2-4)</t>
+  </si>
+  <si>
+    <t>0.5: 0; 0.5: UNIF(0.75 - 1)</t>
+  </si>
+  <si>
+    <t>0.5: 0; 0.5: UNIF(0 - 0.25)</t>
+  </si>
+  <si>
+    <t>if B &gt; 0: UNIF(0 - s)</t>
+  </si>
+  <si>
+    <t>if U &gt; 0: UNIF(-s - 0)</t>
   </si>
 </sst>
 </file>
@@ -623,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC9DF76-A027-4A77-83EC-C4E16205FAC7}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +670,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
         <v>37</v>
@@ -660,13 +684,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,7 +701,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -691,13 +715,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -708,7 +732,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -722,7 +746,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -736,7 +760,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -755,44 +779,44 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D9">
         <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -800,13 +824,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -814,49 +838,55 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -864,21 +894,27 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -886,44 +922,44 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D20">
         <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -931,10 +967,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -942,10 +981,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -953,66 +995,80 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25">
-        <f>PRODUCT(D2:D24)</f>
-        <v>320</v>
-      </c>
-      <c r="E25" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26">
-        <v>1000</v>
+        <f>PRODUCT(D2:D25)</f>
+        <v>320</v>
       </c>
       <c r="E26" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27">
-        <f>PRODUCT(D25:D26)</f>
-        <v>320000</v>
+        <v>1000</v>
       </c>
       <c r="E27" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28">
+        <f>PRODUCT(D26:D27)</f>
+        <v>320000</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29">
         <f>2*1000000</f>
         <v>2000000</v>
       </c>
-      <c r="E28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D29">
+      <c r="E29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30">
         <f>(10000 - 100)/LN(10000/100)</f>
         <v>2149.7576854210965</v>
       </c>
-      <c r="E29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D30">
-        <f>PRODUCT(D27:D29)</f>
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f>PRODUCT(D28:D30)</f>
         <v>1375844918669501.8</v>
       </c>
-      <c r="E30" t="s">
-        <v>66</v>
+      <c r="E31" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update parameter ranges, fix time tracking
</commit_message>
<xml_diff>
--- a/doc/simulation_params_range.xlsx
+++ b/doc/simulation_params_range.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/67802_2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\3279316_2_53\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{3D1C696C-EAB1-46BA-9A69-817FF055F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{186B776E-11AB-449A-9FAD-E48E6BF7E0ED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB36270-3FAA-4ABE-B396-C3F49286B28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t>N</t>
   </si>
@@ -191,15 +191,9 @@
     <t>UNIF(0 - 1)</t>
   </si>
   <si>
-    <t>10^UNIF(-9 - -7)</t>
-  </si>
-  <si>
     <t>UNIF(0-1)</t>
   </si>
   <si>
-    <t>if growing: UNIF(1.5 - 2)*N ; if shrinking: 1/UNIF(1.5-2)*N ; if 2-cycling: UNIF() ; if chaotic: UNIF()</t>
-  </si>
-  <si>
     <t>1 - B - U</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>Number of classes is 1 because the value of K depends on the class of r</t>
   </si>
   <si>
-    <t>10^UNIF(2 - 4)</t>
-  </si>
-  <si>
     <t>Total number of classes</t>
   </si>
   <si>
@@ -266,9 +257,6 @@
     <t>0.5: 1; 0.5: sample(2-4)</t>
   </si>
   <si>
-    <t>0.5: 0; 0.5: UNIF(0.75 - 1)</t>
-  </si>
-  <si>
     <t>0.5: 0; 0.5: UNIF(0 - 0.25)</t>
   </si>
   <si>
@@ -276,6 +264,24 @@
   </si>
   <si>
     <t>if U &gt; 0: UNIF(-s - 0)</t>
+  </si>
+  <si>
+    <t>0.5: 1; 0.5: UNIF(0.75 - 1)</t>
+  </si>
+  <si>
+    <t>10^UNIF(1 - 4)</t>
+  </si>
+  <si>
+    <t>UNIF(1000 - 10000)</t>
+  </si>
+  <si>
+    <t>10^UNIF(-8 - -7)</t>
+  </si>
+  <si>
+    <t>10^UNIF(-10 - -6) or UNIF(0 - 0.25)/(4*N)</t>
+  </si>
+  <si>
+    <t>if growing: UNIF(1.01 - 2)*N ; if shrinking: 1/UNIF(1.01-2)*N ; if 2-cycling: N; if chaotic: N</t>
   </si>
 </sst>
 </file>
@@ -650,7 +656,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +676,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
         <v>37</v>
@@ -684,13 +690,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -715,13 +721,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,7 +738,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -746,7 +752,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -760,7 +766,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -779,13 +785,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -799,13 +805,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -816,7 +822,7 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -844,7 +850,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -858,7 +864,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -872,7 +878,7 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -886,7 +892,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -911,10 +917,10 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -928,7 +934,7 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -942,7 +948,7 @@
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -987,7 +993,7 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1001,7 +1007,7 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1024,7 +1030,7 @@
         <v>320</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1032,7 +1038,7 @@
         <v>1000</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1041,7 +1047,7 @@
         <v>320000</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,7 +1056,7 @@
         <v>2000000</v>
       </c>
       <c r="E29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1059,7 +1065,7 @@
         <v>2149.7576854210965</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1068,7 +1074,7 @@
         <v>1375844918669501.8</v>
       </c>
       <c r="E31" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculate harmonic mean of Ne between burn-in and fixation
</commit_message>
<xml_diff>
--- a/doc/simulation_params_range.xlsx
+++ b/doc/simulation_params_range.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\3279316_2_53\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/197808_2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB36270-3FAA-4ABE-B396-C3F49286B28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4FB36270-3FAA-4ABE-B396-C3F49286B28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71698DC2-BCD4-4392-8941-0BFE98CD691B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -230,9 +230,6 @@
     <t>Ensures about half of coefficients are s &lt; 1/N and the other half are s &gt; 1/N</t>
   </si>
   <si>
-    <t>0.5: 10^UNIF(-3, 0)/N ; 0.5: 10^UNIF(0,3)/N or 10^UNIF(-3,3)/N</t>
-  </si>
-  <si>
     <t>0.5: 0; 0.5:UNIF(0-1)</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>if growing: UNIF(1.01 - 2)*N ; if shrinking: 1/UNIF(1.01-2)*N ; if 2-cycling: N; if chaotic: N</t>
+  </si>
+  <si>
+    <t>0.5: 10^UNIF(-3, 0)/N ; 0.5: 10^UNIF(0,3)/N or 10^UNIF(-3,3)/N or 10^UNIF(-6,0)</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +690,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -721,7 +721,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -738,7 +738,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -752,7 +752,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -785,13 +785,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>70</v>
-      </c>
-      <c r="C9" t="s">
-        <v>71</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -805,7 +805,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -822,7 +822,7 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -836,7 +836,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -850,7 +850,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -864,7 +864,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -878,7 +878,7 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -892,7 +892,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -920,7 +920,7 @@
         <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -934,7 +934,7 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -993,7 +993,7 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1007,7 +1007,7 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24">
         <v>1</v>

</xml_diff>

<commit_message>
try simulations where age of sweep varies
</commit_message>
<xml_diff>
--- a/doc/simulation_params_range.xlsx
+++ b/doc/simulation_params_range.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/197808_2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/66496_2_8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4FB36270-3FAA-4ABE-B396-C3F49286B28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71698DC2-BCD4-4392-8941-0BFE98CD691B}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{4FB36270-3FAA-4ABE-B396-C3F49286B28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E22CEAB-D566-40BD-83AD-7DA74BB48C72}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
+    <workbookView xWindow="20280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="116">
   <si>
     <t>N</t>
   </si>
@@ -282,14 +283,124 @@
   </si>
   <si>
     <t>0.5: 10^UNIF(-3, 0)/N ; 0.5: 10^UNIF(0,3)/N or 10^UNIF(-3,3)/N or 10^UNIF(-6,0)</t>
+  </si>
+  <si>
+    <t>Simulation 1</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Number from 1:K, used as a unique ID for each simulation</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>scaling factor</t>
+  </si>
+  <si>
+    <t>ancestral population size, used for burn-in</t>
+  </si>
+  <si>
+    <t>sweepS</t>
+  </si>
+  <si>
+    <t>selection coefficient for sweep mutation</t>
+  </si>
+  <si>
+    <t>dominance coefficient of sweep mutation</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>time when sweep is introduced (simulation will restart here if sweep fails)</t>
+  </si>
+  <si>
+    <t>threshold frequency to convert sweep from neutral -&gt; beneficial (for soft sweeps)</t>
+  </si>
+  <si>
+    <t>threshold frequency to convert sweep from beneficial -&gt; neutral (for partial sweeps)</t>
+  </si>
+  <si>
+    <t>number of sweep mutations to introduce (recurrent mutation)</t>
+  </si>
+  <si>
+    <t>average waiting time between sweep mutations (poisson distribution)</t>
+  </si>
+  <si>
+    <t>proportion of cross over events that are gene conversions</t>
+  </si>
+  <si>
+    <t>length of gene conversion crossover events</t>
+  </si>
+  <si>
+    <t>fraction of crossover events that are simple</t>
+  </si>
+  <si>
+    <t>proportion of non-sweep mutations that are beneficial</t>
+  </si>
+  <si>
+    <t>proportion of non-sweep mutations that are deleterious</t>
+  </si>
+  <si>
+    <t>proportion of non-sweep mutations that are neutral</t>
+  </si>
+  <si>
+    <t>dominance coefficient for deleterious non-sweep mutations</t>
+  </si>
+  <si>
+    <t>dominance coefficient for beneficial non-sweep mutations</t>
+  </si>
+  <si>
+    <t>bBar</t>
+  </si>
+  <si>
+    <t>average selection coefficient for beneficial non-sweep mutations</t>
+  </si>
+  <si>
+    <t>uBar</t>
+  </si>
+  <si>
+    <t>average selection coefficient for deleterious non-sweep mutations</t>
+  </si>
+  <si>
+    <t>shape parameter for distribution of fitness effects for deleterious non-sweep mutations</t>
+  </si>
+  <si>
+    <t>10^UNIF(-3,0)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Simulation 2</t>
+  </si>
+  <si>
+    <t>number of generations after fixation when sweep is sampled</t>
+  </si>
+  <si>
+    <t>10^UNIF(0,3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -317,8 +428,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC9DF76-A027-4A77-83EC-C4E16205FAC7}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,4 +1198,381 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A1943F-5867-466C-8E64-7A6BA02841CB}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1E-8</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1E-8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
write function to evaluate abc same as cnn
</commit_message>
<xml_diff>
--- a/doc/simulation_params_range.xlsx
+++ b/doc/simulation_params_range.xlsx
@@ -1,43 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\66772_3_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TGSguest\AppData\Local\Temp\Mxt242\RemoteFiles\132230_3_9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95307CA-821D-4AF1-8254-4554B2C16892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FEDE87-AE6C-4A89-AC89-893C1EE4179C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="125">
   <si>
     <t>N</t>
   </si>
@@ -400,13 +389,25 @@
   </si>
   <si>
     <t>constant</t>
+  </si>
+  <si>
+    <t>shrinking</t>
+  </si>
+  <si>
+    <t>growing</t>
+  </si>
+  <si>
+    <t>cycling</t>
+  </si>
+  <si>
+    <t>chaotic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -792,13 +793,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="73" customWidth="1"/>
-    <col min="3" max="4" width="17.140625" customWidth="1"/>
+    <col min="3" max="4" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -815,7 +816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -832,7 +833,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -846,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -863,7 +864,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -877,7 +878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -891,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -905,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -916,7 +917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -930,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -947,7 +948,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -961,7 +962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -975,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -989,7 +990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1003,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1059,7 +1060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1073,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1118,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1157,7 +1158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="D26">
         <f>PRODUCT(D2:D25)</f>
         <v>320</v>
@@ -1166,7 +1167,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="D27">
         <v>1000</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="D28">
         <f>PRODUCT(D26:D27)</f>
         <v>320000</v>
@@ -1183,7 +1184,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="D29">
         <f>2*1000000</f>
         <v>2000000</v>
@@ -1192,7 +1193,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="D30">
         <f>(10000 - 100)/LN(10000/100)</f>
         <v>2149.7576854210965</v>
@@ -1201,7 +1202,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="D31">
         <f>PRODUCT(D28:D30)</f>
         <v>1375844918669501.8</v>
@@ -1217,21 +1218,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A1943F-5867-466C-8E64-7A6BA02841CB}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.4375" customWidth="1"/>
+    <col min="2" max="2" width="39.5625" customWidth="1"/>
+    <col min="3" max="4" width="13.875" customWidth="1"/>
+    <col min="5" max="5" width="12.5625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.9">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1248,7 +1249,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="27">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -1265,7 +1266,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>119</v>
       </c>
@@ -1279,8 +1280,23 @@
       <c r="E3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -1297,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1330,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -1331,7 +1347,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1348,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1365,7 +1381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -1382,7 +1398,7 @@
         <v>1E-8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1399,7 +1415,7 @@
         <v>1E-8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="27">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
@@ -1416,7 +1432,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="27">
       <c r="A12" s="2" t="s">
         <v>92</v>
       </c>
@@ -1433,7 +1449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="27">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1450,7 +1466,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="27">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1467,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="27">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1484,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="27">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1501,7 +1517,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="27">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1518,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1535,7 +1551,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1552,7 +1568,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="27">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1569,7 +1585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="27">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1586,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="27">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -1603,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="27">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1620,7 +1636,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="27">
       <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
@@ -1637,7 +1653,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="27">
       <c r="A25" s="2" t="s">
         <v>106</v>
       </c>
@@ -1654,7 +1670,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="27">
       <c r="A26" s="2" t="s">
         <v>108</v>
       </c>
@@ -1671,7 +1687,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="27">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
create parameter table for growth sims
</commit_message>
<xml_diff>
--- a/doc/simulation_params_range.xlsx
+++ b/doc/simulation_params_range.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TGSguest\AppData\Local\Temp\Mxt242\RemoteFiles\132230_3_9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/133170_2_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FEDE87-AE6C-4A89-AC89-893C1EE4179C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{80FEDE87-AE6C-4A89-AC89-893C1EE4179C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65EAB8B8-0C31-4A43-938A-81058BF3635A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
+    <workbookView xWindow="20280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1E38EC76-5351-4A36-96DC-8C95D5714ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="134">
   <si>
     <t>N</t>
   </si>
@@ -401,13 +412,40 @@
   </si>
   <si>
     <t>chaotic</t>
+  </si>
+  <si>
+    <t>1000:10000</t>
+  </si>
+  <si>
+    <t>UNIF(0,1)</t>
+  </si>
+  <si>
+    <t>10^UNIF(1/N, 0)</t>
+  </si>
+  <si>
+    <t>10^runif(K, min = -8.5, max = -7.5)</t>
+  </si>
+  <si>
+    <t>10^runif(K, min = -9, max = -7)</t>
+  </si>
+  <si>
+    <t>round(10^runif(K, min = 0, max = 4))</t>
+  </si>
+  <si>
+    <t>pattern of how N changed over generations</t>
+  </si>
+  <si>
+    <t>growth</t>
+  </si>
+  <si>
+    <t>decay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,13 +831,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="73" customWidth="1"/>
-    <col min="3" max="4" width="17.125" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -816,7 +854,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -833,7 +871,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -847,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -864,7 +902,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -878,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -892,7 +930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -906,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -917,7 +955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -931,7 +969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -948,7 +986,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -962,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -976,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -990,7 +1028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1004,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1018,7 +1056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1032,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1046,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1060,7 +1098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1074,7 +1112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1091,7 +1129,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1105,7 +1143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1119,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1133,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1147,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1158,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26">
         <f>PRODUCT(D2:D25)</f>
         <v>320</v>
@@ -1167,7 +1205,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>1000</v>
       </c>
@@ -1175,7 +1213,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28">
         <f>PRODUCT(D26:D27)</f>
         <v>320000</v>
@@ -1184,7 +1222,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29">
         <f>2*1000000</f>
         <v>2000000</v>
@@ -1193,7 +1231,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30">
         <f>(10000 - 100)/LN(10000/100)</f>
         <v>2149.7576854210965</v>
@@ -1202,7 +1240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D31">
         <f>PRODUCT(D28:D30)</f>
         <v>1375844918669501.8</v>
@@ -1218,21 +1256,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A1943F-5867-466C-8E64-7A6BA02841CB}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.4375" customWidth="1"/>
-    <col min="2" max="2" width="39.5625" customWidth="1"/>
-    <col min="3" max="4" width="13.875" customWidth="1"/>
-    <col min="5" max="5" width="12.5625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.9">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1245,11 +1283,17 @@
       <c r="D1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="27">
+    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -1259,44 +1303,64 @@
       <c r="C2" t="s">
         <v>117</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
         <v>117</v>
       </c>
-      <c r="E2" t="s">
+      <c r="L2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="M2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="C3" t="s">
         <v>120</v>
       </c>
       <c r="D3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" t="s">
         <v>120</v>
       </c>
-      <c r="E3" t="s">
+      <c r="L3" t="s">
         <v>120</v>
       </c>
-      <c r="F3" t="s">
+      <c r="M3" t="s">
         <v>120</v>
       </c>
-      <c r="G3" t="s">
+      <c r="N3" t="s">
+        <v>120</v>
+      </c>
+      <c r="O3" t="s">
         <v>121</v>
       </c>
-      <c r="H3" t="s">
+      <c r="P3" t="s">
         <v>122</v>
       </c>
-      <c r="I3" t="s">
+      <c r="Q3" t="s">
         <v>123</v>
       </c>
-      <c r="J3" t="s">
+      <c r="R3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>86</v>
       </c>
@@ -1306,31 +1370,37 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K5">
         <v>1000</v>
       </c>
-      <c r="D5">
+      <c r="L5">
         <v>1000</v>
       </c>
-      <c r="E5">
+      <c r="M5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -1338,33 +1408,39 @@
         <v>90</v>
       </c>
       <c r="C6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K6" t="s">
         <v>111</v>
       </c>
-      <c r="D6" t="s">
+      <c r="L6" t="s">
         <v>111</v>
       </c>
-      <c r="E6" t="s">
+      <c r="M6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1372,67 +1448,79 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+      <c r="K9" s="3">
         <v>1E-8</v>
       </c>
-      <c r="D9" s="3">
+      <c r="L9" s="3">
         <v>1E-8</v>
       </c>
-      <c r="E9" s="3">
+      <c r="M9" s="3">
         <v>1E-8</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
+      <c r="K10" s="3">
         <v>1E-8</v>
       </c>
-      <c r="D10" s="3">
+      <c r="L10" s="3">
         <v>1E-8</v>
       </c>
-      <c r="E10" s="3">
+      <c r="M10" s="3">
         <v>1E-8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="27">
+    <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
         <v>115</v>
       </c>
-      <c r="E11" t="s">
+      <c r="M11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="27">
+    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>92</v>
       </c>
@@ -1442,14 +1530,17 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="27">
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1459,14 +1550,17 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13">
+      <c r="K13">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="27">
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1476,14 +1570,17 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="27">
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1493,14 +1590,17 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="27">
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1510,14 +1610,17 @@
       <c r="C16" t="s">
         <v>112</v>
       </c>
-      <c r="D16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="27">
+      <c r="K16" t="s">
+        <v>112</v>
+      </c>
+      <c r="L16" t="s">
+        <v>112</v>
+      </c>
+      <c r="M16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1527,14 +1630,17 @@
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17">
+      <c r="K17">
         <v>0</v>
       </c>
-      <c r="E17">
+      <c r="L17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1544,14 +1650,17 @@
       <c r="C18" t="s">
         <v>112</v>
       </c>
-      <c r="D18" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="K18" t="s">
+        <v>112</v>
+      </c>
+      <c r="L18" t="s">
+        <v>112</v>
+      </c>
+      <c r="M18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1561,14 +1670,17 @@
       <c r="C19" t="s">
         <v>112</v>
       </c>
-      <c r="D19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="27">
+      <c r="K19" t="s">
+        <v>112</v>
+      </c>
+      <c r="L19" t="s">
+        <v>112</v>
+      </c>
+      <c r="M19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1578,14 +1690,17 @@
       <c r="C20">
         <v>0</v>
       </c>
-      <c r="D20">
+      <c r="K20">
         <v>0</v>
       </c>
-      <c r="E20">
+      <c r="L20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="27">
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1595,14 +1710,17 @@
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="D21">
+      <c r="K21">
         <v>0</v>
       </c>
-      <c r="E21">
+      <c r="L21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="27">
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -1612,14 +1730,17 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="27">
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1629,14 +1750,17 @@
       <c r="C23" t="s">
         <v>112</v>
       </c>
-      <c r="D23" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="27">
+      <c r="K23" t="s">
+        <v>112</v>
+      </c>
+      <c r="L23" t="s">
+        <v>112</v>
+      </c>
+      <c r="M23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
@@ -1646,14 +1770,17 @@
       <c r="C24" t="s">
         <v>112</v>
       </c>
-      <c r="D24" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="27">
+      <c r="K24" t="s">
+        <v>112</v>
+      </c>
+      <c r="L24" t="s">
+        <v>112</v>
+      </c>
+      <c r="M24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>106</v>
       </c>
@@ -1663,14 +1790,17 @@
       <c r="C25" t="s">
         <v>112</v>
       </c>
-      <c r="D25" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="27">
+      <c r="K25" t="s">
+        <v>112</v>
+      </c>
+      <c r="L25" t="s">
+        <v>112</v>
+      </c>
+      <c r="M25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>108</v>
       </c>
@@ -1680,14 +1810,17 @@
       <c r="C26" t="s">
         <v>112</v>
       </c>
-      <c r="D26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="27">
+      <c r="K26" t="s">
+        <v>112</v>
+      </c>
+      <c r="L26" t="s">
+        <v>112</v>
+      </c>
+      <c r="M26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
@@ -1697,10 +1830,13 @@
       <c r="C27" t="s">
         <v>112</v>
       </c>
-      <c r="D27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="K27" t="s">
+        <v>112</v>
+      </c>
+      <c r="L27" t="s">
+        <v>112</v>
+      </c>
+      <c r="M27" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>